<commit_message>
CONCLUÍDO - EXERCICIO 4 - SE ENCADEADO FATEC
</commit_message>
<xml_diff>
--- a/[02]-exercicios-fatec/EXERCICIO 4 - SE ENCADEADO.xlsx
+++ b/[02]-exercicios-fatec/EXERCICIO 4 - SE ENCADEADO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Programação em Microinformática\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duanl\Documents\Curso em Vídeo\curso-de-excel-40-horas\[02]-exercicios-fatec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8FB651B-DBEE-4633-812F-C2573ABDE142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FFD8F-8060-4F3E-B7C2-8817205AA49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -678,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2382,7 +2393,10 @@
       <c r="H41" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="9"/>
+      <c r="I41" s="9">
+        <f>SUMIF($B$7:$B$38,H41,$D$7:$D$38)</f>
+        <v>51800</v>
+      </c>
       <c r="J41" s="12"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2405,7 +2419,10 @@
       <c r="H42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I42" s="9"/>
+      <c r="I42" s="9">
+        <f>SUMIF($B$7:$B$38,H42,$D$7:$D$38)</f>
+        <v>33875</v>
+      </c>
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -2428,7 +2445,10 @@
       <c r="H43" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="9"/>
+      <c r="I43" s="9">
+        <f t="shared" ref="I42:I44" si="7">SUMIF($B$7:$B$38,H43,$D$7:$D$38)</f>
+        <v>16700</v>
+      </c>
       <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -2443,12 +2463,18 @@
       <c r="E44" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F44" s="9"/>
+      <c r="F44" s="9">
+        <f>SUM(J7:J38)</f>
+        <v>95355.099999999977</v>
+      </c>
       <c r="G44" s="12"/>
       <c r="H44" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I44" s="9"/>
+      <c r="I44" s="9">
+        <f t="shared" si="7"/>
+        <v>23100</v>
+      </c>
       <c r="J44" s="12"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>